<commit_message>
FF data récolté - 20-09-19
</commit_message>
<xml_diff>
--- a/LRIMA-NezInformatique/results/DL4J-Results.xlsx
+++ b/LRIMA-NezInformatique/results/DL4J-Results.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
@@ -1631,6 +1631,238 @@
         <v>0</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E44" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.30176211453744495</v>
+      </c>
+      <c r="H44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E45" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.2472466960352423</v>
+      </c>
+      <c r="H45" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E46" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.5275330396475771</v>
+      </c>
+      <c r="H46" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E47" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.6227973568281938</v>
+      </c>
+      <c r="H47" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E48" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.8012114537444934</v>
+      </c>
+      <c r="H48" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="B49" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E49" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.8700440528634361</v>
+      </c>
+      <c r="H49" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="B50" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E50" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.9416299559471366</v>
+      </c>
+      <c r="H50" t="n">
+        <v>316.0</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="B51" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E51" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.9564977973568282</v>
+      </c>
+      <c r="H51" t="n">
+        <v>490.0</v>
+      </c>
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Edge Crop Start - 03-10-19
</commit_message>
<xml_diff>
--- a/LRIMA-NezInformatique/results/DL4J-Results.xlsx
+++ b/LRIMA-NezInformatique/results/DL4J-Results.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_bla\Documents\GitHub\LRIMA\LRIMA-NezInformatique\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Surface\Documents\GitHub\LRIMA\LRIMA-NezInformatique\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6F3CD76A-A36D-4EA2-88B1-84583370F471}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CCE48D-24F6-4043-AC0F-1F5B009E33E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15000" windowWidth="19440" xWindow="28680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" r:id="rId1" sheetId="1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$F$44:$F$51</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$G$44:$G$51</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$G$7:$G$15</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -64,7 +69,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,16 +96,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -113,15 +117,1242 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Graphique</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de la précision de l'algorithme (sur 1) en fonction du temps d'entraînement (en secondes)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>A (ANN)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$H$44:$H$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>490</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$G$44:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.30176211453744495</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2472466960352423</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52753303964757714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.62279735682819382</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80121145374449343</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.87004405286343611</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94162995594713661</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.95649779735682816</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DDE3-4061-B39E-F4EF1BC67421}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>B (CNN)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$H$7:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>812</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1083</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1377</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1516</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1688</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1780</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$G$7:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.94202537944762377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8258273202289127</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96964419009703906</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96242846479223687</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97088828066683253</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80666832545409306</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97063946255287381</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97287882557850214</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96317491913411302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DDE3-4061-B39E-F4EF1BC67421}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1329734432"/>
+        <c:axId val="1727000320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1329734432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Temps d'entraînement</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-CA" baseline="0"/>
+                  <a:t> (en s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1727000320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1727000320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Précision</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-CA" baseline="0"/>
+                  <a:t> (sur 1)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1329734432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>211930</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>54766</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Graphique 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87903695-FC63-4CDC-84D0-10A674F4BC09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -156,7 +1387,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -191,7 +1422,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -285,21 +1516,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -316,7 +1547,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -368,23 +1599,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,7 +1644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>3</v>
       </c>
@@ -442,7 +1673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>3</v>
       </c>
@@ -471,7 +1702,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -500,7 +1731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -529,7 +1760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3</v>
       </c>
@@ -558,7 +1789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>3</v>
       </c>
@@ -587,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>3</v>
       </c>
@@ -616,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>3</v>
       </c>
@@ -645,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>3</v>
       </c>
@@ -674,7 +1905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>3</v>
       </c>
@@ -703,7 +1934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>3</v>
       </c>
@@ -732,7 +1963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>3</v>
       </c>
@@ -761,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>3</v>
       </c>
@@ -790,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>3</v>
       </c>
@@ -819,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>3</v>
       </c>
@@ -848,7 +2079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>3</v>
       </c>
@@ -877,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>3</v>
       </c>
@@ -906,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>3</v>
       </c>
@@ -935,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>3</v>
       </c>
@@ -964,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>3</v>
       </c>
@@ -993,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1022,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1051,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1080,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1109,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1138,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1167,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1196,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1225,7 +2456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1254,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1283,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1312,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1341,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1370,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1399,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1428,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1457,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1486,7 +2717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1515,7 +2746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>3</v>
       </c>
@@ -1544,7 +2775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>3</v>
       </c>
@@ -1573,7 +2804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>3</v>
       </c>
@@ -1602,268 +2833,269 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B43" t="n">
-        <v>23.0</v>
-      </c>
-      <c r="C43" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E43" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="F43" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0.9706394625528738</v>
-      </c>
-      <c r="H43" t="n">
-        <v>3973.0</v>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>23</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>50</v>
+      </c>
+      <c r="F43">
+        <v>20</v>
+      </c>
+      <c r="G43">
+        <v>0.97063946255287381</v>
+      </c>
+      <c r="H43">
+        <v>3973</v>
       </c>
       <c r="I43" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="B44" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C44" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="E44" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="F44" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G44" t="n">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>30000</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E44">
+        <v>200</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
         <v>0.30176211453744495</v>
       </c>
-      <c r="H44" t="n">
-        <v>2.0</v>
+      <c r="H44">
+        <v>2</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="B45" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C45" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="E45" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="G45" t="n">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>30000</v>
+      </c>
+      <c r="B45">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E45">
+        <v>200</v>
+      </c>
+      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="G45">
         <v>0.2472466960352423</v>
       </c>
-      <c r="H45" t="n">
-        <v>5.0</v>
+      <c r="H45">
+        <v>5</v>
       </c>
       <c r="I45" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="B46" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C46" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D46" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="E46" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="F46" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.5275330396475771</v>
-      </c>
-      <c r="H46" t="n">
-        <v>8.0</v>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>30000</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E46">
+        <v>200</v>
+      </c>
+      <c r="F46">
+        <v>10</v>
+      </c>
+      <c r="G46">
+        <v>0.52753303964757714</v>
+      </c>
+      <c r="H46">
+        <v>8</v>
       </c>
       <c r="I46" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="B47" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C47" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="E47" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="F47" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0.6227973568281938</v>
-      </c>
-      <c r="H47" t="n">
-        <v>14.0</v>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>30000</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E47">
+        <v>200</v>
+      </c>
+      <c r="F47">
+        <v>20</v>
+      </c>
+      <c r="G47">
+        <v>0.62279735682819382</v>
+      </c>
+      <c r="H47">
+        <v>14</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="B48" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C48" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D48" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="E48" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0.8012114537444934</v>
-      </c>
-      <c r="H48" t="n">
-        <v>33.0</v>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>30000</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E48">
+        <v>200</v>
+      </c>
+      <c r="F48">
+        <v>50</v>
+      </c>
+      <c r="G48">
+        <v>0.80121145374449343</v>
+      </c>
+      <c r="H48">
+        <v>33</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="B49" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C49" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D49" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="E49" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="F49" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0.8700440528634361</v>
-      </c>
-      <c r="H49" t="n">
-        <v>64.0</v>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>30000</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E49">
+        <v>200</v>
+      </c>
+      <c r="F49">
+        <v>100</v>
+      </c>
+      <c r="G49">
+        <v>0.87004405286343611</v>
+      </c>
+      <c r="H49">
+        <v>64</v>
       </c>
       <c r="I49" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="B50" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C50" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D50" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="E50" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="F50" t="n">
-        <v>500.0</v>
-      </c>
-      <c r="G50" t="n">
-        <v>0.9416299559471366</v>
-      </c>
-      <c r="H50" t="n">
-        <v>316.0</v>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>30000</v>
+      </c>
+      <c r="B50">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E50">
+        <v>200</v>
+      </c>
+      <c r="F50">
+        <v>500</v>
+      </c>
+      <c r="G50">
+        <v>0.94162995594713661</v>
+      </c>
+      <c r="H50">
+        <v>316</v>
       </c>
       <c r="I50" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="B51" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C51" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D51" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="E51" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="F51" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="G51" t="n">
-        <v>0.9564977973568282</v>
-      </c>
-      <c r="H51" t="n">
-        <v>490.0</v>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>30000</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E51">
+        <v>200</v>
+      </c>
+      <c r="F51">
+        <v>1000</v>
+      </c>
+      <c r="G51">
+        <v>0.95649779735682816</v>
+      </c>
+      <c r="H51">
+        <v>490</v>
       </c>
       <c r="I51" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Fresh-Rotten dataset- 10-07-19
</commit_message>
<xml_diff>
--- a/LRIMA-NezInformatique/results/DL4J-Results.xlsx
+++ b/LRIMA-NezInformatique/results/DL4J-Results.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Surface\Documents\GitHub\LRIMA\LRIMA-NezInformatique\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CCE48D-24F6-4043-AC0F-1F5B009E33E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACA50DE-8B55-4CEB-A3E5-0117FAD06DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Fruit Recognition" sheetId="1" r:id="rId1"/>
+    <sheet name="Fresh-Rotten" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$F$44:$F$51</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$G$44:$G$51</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$G$7:$G$15</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
   <si>
     <t>Number of channels</t>
   </si>
@@ -229,7 +225,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$H$44:$H$51</c:f>
+              <c:f>'Fruit Recognition'!$H$44:$H$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -262,7 +258,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$G$44:$G$51</c:f>
+              <c:f>'Fruit Recognition'!$G$44:$G$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -332,7 +328,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$H$7:$H$15</c:f>
+              <c:f>'Fruit Recognition'!$H$7:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -368,7 +364,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$G$7:$G$15</c:f>
+              <c:f>'Fruit Recognition'!$G$7:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1607,10 +1603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3094,8 +3090,111 @@
         <v>0</v>
       </c>
     </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E056317B-7ABC-4385-A6AC-B9A8BF4C3B46}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>0.86174944403261677</v>
+      </c>
+      <c r="G2">
+        <v>1993</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0.8528539659006672</v>
+      </c>
+      <c r="G3">
+        <v>403</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
UI to recognize - 08-10-2019-1700
</commit_message>
<xml_diff>
--- a/LRIMA-NezInformatique/results/DL4J-Results.xlsx
+++ b/LRIMA-NezInformatique/results/DL4J-Results.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_bla\Documents\GitHub\LRIMA\LRIMA-NezInformatique\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Surface\Documents\GitHub\LRIMA\LRIMA-NezInformatique\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3EC7F0-97D7-494C-9773-26E0573B6D95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{CDD63D4F-7F1F-4BF6-B4D3-AE2482E8AA87}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" windowHeight="13276" windowWidth="20715" xWindow="-98" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-98"/>
   </bookViews>
   <sheets>
-    <sheet name="Fruit Recognition" sheetId="1" r:id="rId1"/>
-    <sheet name="Fresh-Rotten" sheetId="2" r:id="rId2"/>
+    <sheet name="Fruit Recognition" r:id="rId1" sheetId="1"/>
+    <sheet name="Fresh-Rotten" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <si>
     <t>Number of channels</t>
   </si>
@@ -60,11 +60,21 @@
   <si>
     <t>true</t>
   </si>
+  <si>
+    <t>Aliment</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,16 +102,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -114,7 +124,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -130,11 +140,11 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400" u="none">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -151,7 +161,7 @@
               <a:t>Graphique</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr baseline="0" lang="en-US"/>
               <a:t> de la précision de l'algorithme (sur 1) en fonction du temps d'entraînement (en secondes)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
@@ -167,11 +177,11 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400" u="none">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -200,7 +210,7 @@
             <c:v>A (ANN)</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln cap="rnd" w="19050">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -303,7 +313,7 @@
             <c:v>B (CNN)</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln cap="rnd" w="19050">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -425,7 +435,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -440,11 +450,11 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="1000" u="none">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -461,7 +471,7 @@
                   <a:t>Temps d'entraînement</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="fr-CA" baseline="0"/>
+                  <a:rPr baseline="0" lang="fr-CA"/>
                   <a:t> (en s)</a:t>
                 </a:r>
                 <a:endParaRPr lang="fr-CA"/>
@@ -477,11 +487,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="1000" u="none">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -503,7 +513,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="25000"/>
@@ -515,11 +525,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -547,7 +557,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -562,11 +572,11 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr anchor="ctr" anchorCtr="1" rot="-5400000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="1000" u="none">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -583,7 +593,7 @@
                   <a:t>Précision</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="fr-CA" baseline="0"/>
+                  <a:rPr baseline="0" lang="fr-CA"/>
                   <a:t> (sur 1)</a:t>
                 </a:r>
                 <a:endParaRPr lang="fr-CA"/>
@@ -599,11 +609,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr anchor="ctr" anchorCtr="1" rot="-5400000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="1000" u="none">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -625,7 +635,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="25000"/>
@@ -637,11 +647,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -679,11 +689,11 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -714,7 +724,7 @@
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
       <a:solidFill>
         <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
@@ -737,7 +747,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75" footer="0.3" header="0.3" l="0.7" r="0.7" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1300,7 +1310,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -1345,10 +1355,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1383,7 +1393,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -1418,7 +1428,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1512,21 +1522,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1543,7 +1553,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1595,23 +1605,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView topLeftCell="B31" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1640,7 +1650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1669,7 +1679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1698,7 +1708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1727,7 +1737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1756,7 +1766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1785,7 +1795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1814,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1843,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1872,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1901,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1930,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1959,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1988,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2017,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2046,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2075,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2104,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2133,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2162,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2191,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2220,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2249,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2278,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2307,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2336,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2365,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2394,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2423,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2452,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2481,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2510,7 +2520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2539,7 +2549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2568,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2597,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2626,7 +2636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2655,7 +2665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2684,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2713,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2742,7 +2752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2771,7 +2781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2800,7 +2810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2829,7 +2839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2858,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>30000</v>
       </c>
@@ -2887,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>30000</v>
       </c>
@@ -2916,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>30000</v>
       </c>
@@ -2945,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>30000</v>
       </c>
@@ -2974,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>30000</v>
       </c>
@@ -3003,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>30000</v>
       </c>
@@ -3032,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>30000</v>
       </c>
@@ -3061,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>30000</v>
       </c>
@@ -3090,33 +3100,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E056317B-7ABC-4385-A6AC-B9A8BF4C3B46}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E056317B-7ABC-4385-A6AC-B9A8BF4C3B46}">
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3144,8 +3154,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>3</v>
       </c>
@@ -3173,8 +3186,11 @@
       <c r="I2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3202,8 +3218,11 @@
       <c r="I3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3231,8 +3250,136 @@
       <c r="I4" t="b">
         <v>0</v>
       </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0.59337349397590367</v>
+      </c>
+      <c r="H5">
+        <v>344</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>0.91767068273092367</v>
+      </c>
+      <c r="H6">
+        <v>802</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>0.93574297188755018</v>
+      </c>
+      <c r="H7">
+        <v>1165</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.995609220636663</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1195.0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>